<commit_message>
Ajustes finales para despliege
</commit_message>
<xml_diff>
--- a/App/RegistroAsistenciasSMART.Web/Formato/PlantillaColaboradores.xlsx
+++ b/App/RegistroAsistenciasSMART.Web/Formato/PlantillaColaboradores.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usuario\Documents\Fuentes SMART\RegistroAsistencias\App\RegistroAsistenciasSMART.Web\wwwroot\Formatos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Fuentes\FuentesSMART\AsistenciasV2\App\RegistroAsistenciasSMART.Web\Formato\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B04437E-DAE1-4458-B37A-9FE670D7A89B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C771C724-1CAF-4809-9DB3-042B4C79F4BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{01196104-56FC-4D66-A5D6-1A230B06E7A5}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{01196104-56FC-4D66-A5D6-1A230B06E7A5}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>CEDULA</t>
   </si>
@@ -48,22 +48,28 @@
     <t>AREA</t>
   </si>
   <si>
-    <t>JEFE INMEDIATO</t>
-  </si>
-  <si>
     <t>SEDE</t>
   </si>
   <si>
     <t>CORREO</t>
   </si>
   <si>
-    <t>TURNO</t>
-  </si>
-  <si>
-    <t>ESTADO</t>
-  </si>
-  <si>
     <t>APELLIDOS</t>
+  </si>
+  <si>
+    <t>CÉDULA DEL JEFE INMEDIATO</t>
+  </si>
+  <si>
+    <t>HORA DE ENTRADA L-V</t>
+  </si>
+  <si>
+    <t>HORA DE SALIDA L-V</t>
+  </si>
+  <si>
+    <t>HORA DE SALIDA SÁBADOS</t>
+  </si>
+  <si>
+    <t>HORA DE ENTRADA SÁBADOS</t>
   </si>
 </sst>
 </file>
@@ -139,9 +145,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -179,7 +185,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -285,7 +291,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -427,7 +433,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -435,15 +441,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4E3842A-0D05-4E23-B522-263010424B38}">
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="17.26953125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="9" max="9" width="21.28515625" customWidth="1"/>
+    <col min="10" max="10" width="19.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -451,7 +461,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
@@ -460,19 +470,25 @@
         <v>3</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>6</v>
-      </c>
       <c r="I1" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ajuste para permitir parametrizar horarios de los días viernes
</commit_message>
<xml_diff>
--- a/App/RegistroAsistenciasSMART.Web/Formato/PlantillaColaboradores.xlsx
+++ b/App/RegistroAsistenciasSMART.Web/Formato/PlantillaColaboradores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Fuentes\FuentesSMART\AsistenciasV2\App\RegistroAsistenciasSMART.Web\Formato\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C771C724-1CAF-4809-9DB3-042B4C79F4BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{507290B3-0056-416B-BC32-DD84EFD60B7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{01196104-56FC-4D66-A5D6-1A230B06E7A5}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>CEDULA</t>
   </si>
@@ -60,16 +60,22 @@
     <t>CÉDULA DEL JEFE INMEDIATO</t>
   </si>
   <si>
-    <t>HORA DE ENTRADA L-V</t>
-  </si>
-  <si>
-    <t>HORA DE SALIDA L-V</t>
-  </si>
-  <si>
     <t>HORA DE SALIDA SÁBADOS</t>
   </si>
   <si>
     <t>HORA DE ENTRADA SÁBADOS</t>
+  </si>
+  <si>
+    <t>HORA DE ENTRADA L-J</t>
+  </si>
+  <si>
+    <t>HORA DE SALIDA L-J</t>
+  </si>
+  <si>
+    <t>HORA DE ENTRADA VIERNES</t>
+  </si>
+  <si>
+    <t>HORA DE SALIDA VIERNES</t>
   </si>
 </sst>
 </file>
@@ -441,19 +447,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4E3842A-0D05-4E23-B522-263010424B38}">
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:N1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="9" max="9" width="21.28515625" customWidth="1"/>
-    <col min="10" max="10" width="19.42578125" customWidth="1"/>
+    <col min="10" max="12" width="19.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -479,16 +485,22 @@
         <v>5</v>
       </c>
       <c r="I1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="N1" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ajustando columnas de la plantilla de cargue en columnas de horarios
</commit_message>
<xml_diff>
--- a/App/RegistroAsistenciasSMART.Web/Formato/PlantillaColaboradores.xlsx
+++ b/App/RegistroAsistenciasSMART.Web/Formato/PlantillaColaboradores.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Fuentes\FuentesSMART\AsistenciasV2\App\RegistroAsistenciasSMART.Web\Formato\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{507290B3-0056-416B-BC32-DD84EFD60B7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BA65CA7-62B8-4F3C-8D51-27DF3314CA5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{01196104-56FC-4D66-A5D6-1A230B06E7A5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{01196104-56FC-4D66-A5D6-1A230B06E7A5}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -125,7 +125,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -133,6 +133,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="18" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -450,13 +454,14 @@
   <dimension ref="A1:N1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="N1" activeCellId="5" sqref="I1:I1048576 J1:J1048576 K1:K1048576 L1:L1048576 M1:M1048576 N1:N1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="9" max="9" width="21.28515625" customWidth="1"/>
-    <col min="10" max="12" width="19.42578125" customWidth="1"/>
+    <col min="9" max="9" width="21.28515625" style="4" customWidth="1"/>
+    <col min="10" max="12" width="19.42578125" style="4" customWidth="1"/>
+    <col min="13" max="14" width="17.28515625" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -484,22 +489,22 @@
       <c r="H1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="N1" s="3" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>